<commit_message>
Got this working so far
It is grabbing all the channels, think i can keep going past 21. Going to try then need to make a class to calculate the amps.
</commit_message>
<xml_diff>
--- a/KeeperAmps.xlsx
+++ b/KeeperAmps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/speedy/Documents/GitProjects/AmpSheetRepository/AmpSheetMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A410C6E8-BDC0-304D-A54E-8AF24AD5BCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5B9DAD0-72F6-CC40-AED4-2E530F91E489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33240" yWindow="1960" windowWidth="28040" windowHeight="17440" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20560" xr2:uid="{329AA3C5-52D5-8A41-A20D-B75AE869BCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Racks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="31">
   <si>
     <t>ChanLow</t>
   </si>
@@ -129,12 +129,15 @@
   <si>
     <t>All Sheet Amps</t>
   </si>
+  <si>
+    <t>Voltage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,6 +169,34 @@
     <font>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="2"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -409,11 +440,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -448,12 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,10 +495,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -477,103 +507,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -588,41 +522,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,14 +529,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -649,35 +540,227 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1013,15 +1096,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41DDF0-49AF-A145-B81B-BCD86198E320}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="22">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1049,14 +1136,14 @@
       <c r="I1" s="8"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="22">
       <c r="A2" s="10"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1073,7 +1160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="22">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1086,23 +1173,23 @@
       <c r="D3" s="4">
         <v>3.22</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="4">
         <v>1001</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="22">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="4">
         <v>5.37</v>
       </c>
@@ -1121,11 +1208,11 @@
       <c r="I4" s="4">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="22">
       <c r="A5" s="4"/>
       <c r="B5" s="3">
         <v>3</v>
@@ -1133,7 +1220,7 @@
       <c r="C5" s="4">
         <v>4.58</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="4">
         <v>4.58</v>
       </c>
@@ -1145,9 +1232,9 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="22">
       <c r="A6" s="4"/>
       <c r="B6" s="3">
         <v>4</v>
@@ -1158,7 +1245,7 @@
       <c r="D6" s="4">
         <v>7.66</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="4">
         <v>905</v>
       </c>
@@ -1171,16 +1258,16 @@
       <c r="I6" s="4">
         <v>902</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="12">
         <v>907</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="22">
       <c r="A7" s="4"/>
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="4">
         <v>2.12</v>
       </c>
@@ -1199,11 +1286,11 @@
       <c r="I7" s="4">
         <v>304</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="22">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1300,7 @@
       <c r="C8" s="4">
         <v>3.22</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="4">
         <v>3.22</v>
       </c>
@@ -1223,100 +1310,100 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="22">
+      <c r="A9" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <f>SUM(C3:C8)</f>
         <v>18.68</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <f>SUM(D3:D8)</f>
         <v>18.37</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="15">
         <f>SUM(E3:E8)</f>
         <v>15.290000000000001</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:10" ht="24">
+      <c r="A10" s="32"/>
+      <c r="B10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="70">
         <f>SUM(C9:E9)</f>
         <v>52.339999999999996</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="36">
         <f>ROUNDUP(SUM(C9:E9)/3,2)</f>
         <v>17.450000000000003</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-    </row>
-    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="31">
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:10" ht="22" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="64">
         <f>C10</f>
         <v>52.339999999999996</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34">
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="41">
         <f>G10</f>
         <v>17.450000000000003</v>
       </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="36"/>
-    </row>
-    <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-    </row>
-    <row r="13" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="44"/>
-    </row>
-    <row r="14" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" ht="22" customHeight="1">
+      <c r="A12" s="40"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="46"/>
+    </row>
+    <row r="13" spans="1:10" s="76" customFormat="1" ht="11">
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="75"/>
+    </row>
+    <row r="14" spans="1:10" ht="22">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1344,14 +1431,14 @@
       <c r="I14" s="8"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:10" ht="22">
+      <c r="A15" s="17"/>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="22">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1381,7 +1468,7 @@
       <c r="D16" s="3">
         <v>4.58</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="4">
         <v>804</v>
       </c>
@@ -1390,16 +1477,16 @@
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="22">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="3">
         <v>3.22</v>
       </c>
@@ -1412,9 +1499,9 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="22">
       <c r="A18" s="4"/>
       <c r="B18" s="3">
         <v>3</v>
@@ -1422,7 +1509,7 @@
       <c r="C18" s="3">
         <v>6.13</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="3">
         <v>6.13</v>
       </c>
@@ -1438,9 +1525,9 @@
       <c r="I18" s="4">
         <v>912</v>
       </c>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" ht="22">
       <c r="A19" s="4"/>
       <c r="B19" s="3">
         <v>4</v>
@@ -1451,7 +1538,7 @@
       <c r="D19" s="3">
         <v>1.26</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4">
         <v>7</v>
@@ -1462,14 +1549,14 @@
       <c r="I19" s="4">
         <v>6</v>
       </c>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" ht="22">
       <c r="A20" s="4"/>
       <c r="B20" s="3">
         <v>5</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="3">
         <v>2.12</v>
       </c>
@@ -1488,11 +1575,11 @@
       <c r="I20" s="4">
         <v>310</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="12">
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="22">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1502,7 +1589,7 @@
       <c r="C21" s="3">
         <v>3.22</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="3">
         <v>3.22</v>
       </c>
@@ -1512,90 +1599,90 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="22">
+      <c r="A22" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="18">
         <f>SUM(C16:C21)</f>
         <v>15.190000000000001</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="19">
         <f>SUM(D16:D21)</f>
         <v>11.18</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="20">
         <f>SUM(E16:E21)</f>
         <v>14.69</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23" t="s">
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="1:10" ht="22">
+      <c r="A23" s="32"/>
+      <c r="B23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="57">
         <f>SUM(C22:E22)</f>
         <v>41.06</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="19">
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="33">
         <f>ROUNDUP(SUM(C22:E22)/3,2)</f>
         <v>13.69</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="73" t="s">
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:10" ht="22" customHeight="1">
+      <c r="A24" s="47"/>
+      <c r="B24" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C24" s="49">
         <f>SUM(C11+C23)</f>
         <v>93.4</v>
       </c>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="53">
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="49">
         <f>SUM(G11+G23)</f>
         <v>31.14</v>
       </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
-    </row>
-    <row r="25" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="56"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="59"/>
-    </row>
-    <row r="26" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" ht="22" customHeight="1">
+      <c r="A25" s="48"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
+    </row>
+    <row r="26" spans="1:10" ht="22">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1623,14 +1710,14 @@
       <c r="I26" s="8"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="22">
       <c r="A27" s="10"/>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1647,7 +1734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="22">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1747,7 @@
       <c r="D28" s="4">
         <v>4.58</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="4">
         <v>806</v>
       </c>
@@ -1669,16 +1756,16 @@
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" ht="22">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="4">
         <v>7.66</v>
       </c>
@@ -1697,11 +1784,11 @@
       <c r="I29" s="4">
         <v>918</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="12">
         <v>916</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="22">
       <c r="A30" s="4"/>
       <c r="B30" s="3">
         <v>3</v>
@@ -1709,7 +1796,7 @@
       <c r="C30" s="4">
         <v>1.26</v>
       </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="4">
         <v>1.26</v>
       </c>
@@ -1723,9 +1810,9 @@
         <v>10</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" ht="22">
       <c r="A31" s="4"/>
       <c r="B31" s="3">
         <v>4</v>
@@ -1736,7 +1823,7 @@
       <c r="D31" s="4">
         <v>2.12</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="4">
         <v>312</v>
       </c>
@@ -1749,16 +1836,16 @@
       <c r="I31" s="4">
         <v>314</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="12">
         <v>313</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="22">
       <c r="A32" s="4"/>
       <c r="B32" s="3">
         <v>5</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="4">
         <v>3.22</v>
       </c>
@@ -1771,9 +1858,9 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" ht="22">
       <c r="A33" s="3" t="s">
         <v>12</v>
       </c>
@@ -1783,7 +1870,7 @@
       <c r="C33" s="4">
         <v>3.22</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="4">
         <v>3.22</v>
       </c>
@@ -1793,100 +1880,100 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" ht="22">
+      <c r="A34" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="13">
         <f>SUM(C28:C33)</f>
         <v>11.18</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="14">
         <f>SUM(D28:D33)</f>
         <v>17.579999999999998</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="15">
         <f>SUM(E28:E33)</f>
         <v>15.360000000000001</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="21"/>
-    </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23" t="s">
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="35"/>
+    </row>
+    <row r="35" spans="1:10" ht="24">
+      <c r="A35" s="32"/>
+      <c r="B35" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="70">
         <f>SUM(C34:E34)</f>
         <v>44.12</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27">
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="36">
         <f>ROUNDUP(SUM(C34:E34)/3,2)</f>
         <v>14.709999999999999</v>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="29"/>
-    </row>
-    <row r="36" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="31">
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
+    </row>
+    <row r="36" spans="1:10" ht="22" customHeight="1">
+      <c r="A36" s="39"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="64">
         <f>C35</f>
         <v>44.12</v>
       </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="34">
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="41">
         <f>G35</f>
         <v>14.709999999999999</v>
       </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="36"/>
-    </row>
-    <row r="37" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="43"/>
-    </row>
-    <row r="38" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="44"/>
-    </row>
-    <row r="39" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="43"/>
+    </row>
+    <row r="37" spans="1:10" ht="22" customHeight="1">
+      <c r="A37" s="40"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="46"/>
+    </row>
+    <row r="38" spans="1:10" s="76" customFormat="1" ht="11">
+      <c r="A38" s="73"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
+    </row>
+    <row r="39" spans="1:10" ht="22">
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1914,14 +2001,14 @@
       <c r="I39" s="8"/>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A40" s="45"/>
+    <row r="40" spans="1:10" ht="22">
+      <c r="A40" s="17"/>
       <c r="B40" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
       <c r="F40" s="3" t="s">
         <v>9</v>
       </c>
@@ -1934,11 +2021,11 @@
       <c r="I40" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J40" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J40" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="22">
       <c r="A41" s="3" t="s">
         <v>10</v>
       </c>
@@ -1951,7 +2038,7 @@
       <c r="D41" s="3">
         <v>6.45</v>
       </c>
-      <c r="E41" s="13"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="4">
         <v>1008</v>
       </c>
@@ -1960,16 +2047,16 @@
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" ht="22">
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="3">
         <v>2</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="3">
         <v>3.11</v>
       </c>
@@ -1988,11 +2075,11 @@
       <c r="I42" s="4">
         <v>18</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="12">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="22">
       <c r="A43" s="4"/>
       <c r="B43" s="3">
         <v>3</v>
@@ -2000,11 +2087,11 @@
       <c r="C43" s="3">
         <v>5</v>
       </c>
-      <c r="D43" s="13"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="3">
         <v>5</v>
       </c>
-      <c r="F43" s="61">
+      <c r="F43" s="22">
         <v>20</v>
       </c>
       <c r="G43" s="4">
@@ -2014,9 +2101,9 @@
         <v>813</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="J43" s="14"/>
-    </row>
-    <row r="44" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" ht="22">
       <c r="A44" s="4"/>
       <c r="B44" s="3">
         <v>4</v>
@@ -2027,7 +2114,7 @@
       <c r="D44" s="3">
         <v>7.66</v>
       </c>
-      <c r="E44" s="13"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="4">
         <v>939</v>
       </c>
@@ -2040,16 +2127,16 @@
       <c r="I44" s="4">
         <v>938</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="12">
         <v>940</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="22">
       <c r="A45" s="4"/>
       <c r="B45" s="3">
         <v>5</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="3">
         <v>2.12</v>
       </c>
@@ -2068,11 +2155,11 @@
       <c r="I45" s="4">
         <v>331</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="12">
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="22">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
@@ -2082,108 +2169,108 @@
       <c r="C46" s="3">
         <v>0</v>
       </c>
-      <c r="D46" s="13"/>
+      <c r="D46" s="11"/>
       <c r="E46" s="3">
         <v>0</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A47" s="62" t="s">
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="1:10" ht="22">
+      <c r="A47" s="55" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="46">
+      <c r="C47" s="18">
         <f>SUM(C41:C46)</f>
         <v>19.11</v>
       </c>
-      <c r="D47" s="47">
+      <c r="D47" s="19">
         <f>SUM(D41:D46)</f>
         <v>19.34</v>
       </c>
-      <c r="E47" s="48">
+      <c r="E47" s="20">
         <f>SUM(E41:E46)</f>
         <v>10.23</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="21"/>
-    </row>
-    <row r="48" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A48" s="63"/>
-      <c r="B48" s="23" t="s">
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="35"/>
+    </row>
+    <row r="48" spans="1:10" ht="22">
+      <c r="A48" s="56"/>
+      <c r="B48" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="49">
+      <c r="C48" s="57">
         <f>SUM(C47:E47)</f>
         <v>48.680000000000007</v>
       </c>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="19">
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="33">
         <f>ROUNDUP(SUM(C47:E47)/3,2)</f>
         <v>16.23</v>
       </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="21"/>
-    </row>
-    <row r="49" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="52"/>
-      <c r="B49" s="73" t="s">
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="35"/>
+    </row>
+    <row r="49" spans="1:10" ht="22" customHeight="1">
+      <c r="A49" s="47"/>
+      <c r="B49" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="53">
+      <c r="C49" s="49">
         <f>SUM(C36+C48)</f>
         <v>92.800000000000011</v>
       </c>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="53">
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="49">
         <f>SUM(G36+G48)</f>
         <v>30.939999999999998</v>
       </c>
-      <c r="H49" s="54"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="55"/>
-    </row>
-    <row r="50" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="56"/>
-      <c r="B50" s="74"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="59"/>
-    </row>
-    <row r="51" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="44"/>
-    </row>
-    <row r="52" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="51"/>
+    </row>
+    <row r="50" spans="1:10" ht="22" customHeight="1">
+      <c r="A50" s="48"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="54"/>
+    </row>
+    <row r="51" spans="1:10" s="76" customFormat="1" ht="11">
+      <c r="A51" s="73"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
+      <c r="J51" s="75"/>
+    </row>
+    <row r="52" spans="1:10" ht="22">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
@@ -2211,14 +2298,14 @@
       <c r="I52" s="8"/>
       <c r="J52" s="9"/>
     </row>
-    <row r="53" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="22">
       <c r="A53" s="10"/>
       <c r="B53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
       <c r="F53" s="3" t="s">
         <v>9</v>
       </c>
@@ -2235,7 +2322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="22">
       <c r="A54" s="4"/>
       <c r="B54" s="3">
         <v>1</v>
@@ -2246,25 +2333,25 @@
       <c r="D54" s="4">
         <v>5.51</v>
       </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="64">
+      <c r="E54" s="11"/>
+      <c r="F54" s="23">
         <v>816</v>
       </c>
-      <c r="G54" s="64">
+      <c r="G54" s="23">
         <v>1010</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="14"/>
-    </row>
-    <row r="55" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="1:10" ht="22">
       <c r="A55" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B55" s="3">
         <v>2</v>
       </c>
-      <c r="C55" s="13"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="4">
         <v>5.51</v>
       </c>
@@ -2279,9 +2366,9 @@
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="14"/>
-    </row>
-    <row r="56" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="1:10" ht="22">
       <c r="A56" s="3" t="s">
         <v>11</v>
       </c>
@@ -2291,7 +2378,7 @@
       <c r="C56" s="4">
         <v>6.13</v>
       </c>
-      <c r="D56" s="13"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="4">
         <v>6.13</v>
       </c>
@@ -2307,9 +2394,9 @@
       <c r="I56" s="4">
         <v>947</v>
       </c>
-      <c r="J56" s="14"/>
-    </row>
-    <row r="57" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J56" s="12"/>
+    </row>
+    <row r="57" spans="1:10" ht="22">
       <c r="A57" s="4"/>
       <c r="B57" s="3">
         <v>4</v>
@@ -2320,25 +2407,25 @@
       <c r="D57" s="4">
         <v>1.26</v>
       </c>
-      <c r="E57" s="13"/>
-      <c r="F57" s="64">
+      <c r="E57" s="11"/>
+      <c r="F57" s="23">
         <v>14</v>
       </c>
-      <c r="G57" s="64"/>
-      <c r="H57" s="64">
+      <c r="G57" s="23"/>
+      <c r="H57" s="23">
         <v>16</v>
       </c>
-      <c r="I57" s="64">
+      <c r="I57" s="23">
         <v>15</v>
       </c>
-      <c r="J57" s="14"/>
-    </row>
-    <row r="58" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J57" s="12"/>
+    </row>
+    <row r="58" spans="1:10" ht="22">
       <c r="A58" s="4"/>
       <c r="B58" s="3">
         <v>5</v>
       </c>
-      <c r="C58" s="13"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="4">
         <v>2.12</v>
       </c>
@@ -2357,11 +2444,11 @@
       <c r="I58" s="4">
         <v>338</v>
       </c>
-      <c r="J58" s="14">
+      <c r="J58" s="12">
         <v>337</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="22">
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +2458,7 @@
       <c r="C59" s="4">
         <v>0</v>
       </c>
-      <c r="D59" s="13"/>
+      <c r="D59" s="11"/>
       <c r="E59" s="4">
         <v>0</v>
       </c>
@@ -2379,100 +2466,100 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="14"/>
-    </row>
-    <row r="60" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A60" s="62" t="s">
+      <c r="J59" s="12"/>
+    </row>
+    <row r="60" spans="1:10" ht="22">
+      <c r="A60" s="55" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="16">
+      <c r="C60" s="13">
         <f>SUM(C54:C59)</f>
         <v>12.9</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="14">
         <f>SUM(D54:D59)</f>
         <v>14.399999999999999</v>
       </c>
-      <c r="E60" s="18">
+      <c r="E60" s="15">
         <f>SUM(E54:E59)</f>
         <v>13.760000000000002</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="21"/>
-    </row>
-    <row r="61" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="63"/>
-      <c r="B61" s="23" t="s">
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="35"/>
+    </row>
+    <row r="61" spans="1:10" ht="24">
+      <c r="A61" s="56"/>
+      <c r="B61" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="70">
         <f>SUM(C60:E60)</f>
         <v>41.06</v>
       </c>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="27">
+      <c r="D61" s="71"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="36">
         <f>ROUNDUP(SUM(C60:E60)/3,2)</f>
         <v>13.69</v>
       </c>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="29"/>
-    </row>
-    <row r="62" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="31">
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="38"/>
+    </row>
+    <row r="62" spans="1:10" ht="22" customHeight="1">
+      <c r="A62" s="39"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="64">
         <f>C61</f>
         <v>41.06</v>
       </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="34">
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="41">
         <f>G61</f>
         <v>13.69</v>
       </c>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="36"/>
-    </row>
-    <row r="63" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="37"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="42"/>
-      <c r="J63" s="43"/>
-    </row>
-    <row r="64" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A64" s="11"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="44"/>
-    </row>
-    <row r="65" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H62" s="42"/>
+      <c r="I62" s="42"/>
+      <c r="J62" s="43"/>
+    </row>
+    <row r="63" spans="1:10" ht="22" customHeight="1">
+      <c r="A63" s="40"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="46"/>
+    </row>
+    <row r="64" spans="1:10" s="76" customFormat="1" ht="11">
+      <c r="A64" s="73"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
+      <c r="F64" s="74"/>
+      <c r="G64" s="74"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="74"/>
+      <c r="J64" s="75"/>
+    </row>
+    <row r="65" spans="1:10" ht="22">
       <c r="A65" s="3" t="s">
         <v>3</v>
       </c>
@@ -2500,14 +2587,14 @@
       <c r="I65" s="8"/>
       <c r="J65" s="9"/>
     </row>
-    <row r="66" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A66" s="45"/>
+    <row r="66" spans="1:10" ht="22">
+      <c r="A66" s="17"/>
       <c r="B66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
       <c r="F66" s="3" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="22">
       <c r="A67" s="4"/>
       <c r="B67" s="3">
         <v>1</v>
@@ -2535,7 +2622,7 @@
       <c r="D67" s="3">
         <v>4.58</v>
       </c>
-      <c r="E67" s="13"/>
+      <c r="E67" s="11"/>
       <c r="F67" s="4">
         <v>818</v>
       </c>
@@ -2544,16 +2631,16 @@
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="14"/>
-    </row>
-    <row r="68" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J67" s="12"/>
+    </row>
+    <row r="68" spans="1:10" ht="22">
       <c r="A68" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B68" s="3">
         <v>2</v>
       </c>
-      <c r="C68" s="13"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="3">
         <v>7.66</v>
       </c>
@@ -2572,11 +2659,11 @@
       <c r="I68" s="4">
         <v>952</v>
       </c>
-      <c r="J68" s="14">
+      <c r="J68" s="12">
         <v>951</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="22">
       <c r="A69" s="3" t="s">
         <v>11</v>
       </c>
@@ -2586,7 +2673,7 @@
       <c r="C69" s="3">
         <v>1.26</v>
       </c>
-      <c r="D69" s="13"/>
+      <c r="D69" s="11"/>
       <c r="E69" s="3">
         <v>1.26</v>
       </c>
@@ -2600,9 +2687,9 @@
       <c r="I69" s="4">
         <v>11</v>
       </c>
-      <c r="J69" s="14"/>
-    </row>
-    <row r="70" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="J69" s="12"/>
+    </row>
+    <row r="70" spans="1:10" ht="22">
       <c r="A70" s="4"/>
       <c r="B70" s="3">
         <v>4</v>
@@ -2613,29 +2700,29 @@
       <c r="D70" s="3">
         <v>2.12</v>
       </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="64">
+      <c r="E70" s="11"/>
+      <c r="F70" s="23">
         <v>340</v>
       </c>
-      <c r="G70" s="64">
+      <c r="G70" s="23">
         <v>341</v>
       </c>
-      <c r="H70" s="65">
+      <c r="H70" s="24">
         <v>344</v>
       </c>
-      <c r="I70" s="65">
+      <c r="I70" s="24">
         <v>343</v>
       </c>
-      <c r="J70" s="66">
+      <c r="J70" s="25">
         <v>342</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="22">
       <c r="A71" s="4"/>
       <c r="B71" s="3">
         <v>5</v>
       </c>
-      <c r="C71" s="13"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="3">
         <v>6.45</v>
       </c>
@@ -2650,9 +2737,9 @@
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="14"/>
-    </row>
-    <row r="72" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J71" s="12"/>
+    </row>
+    <row r="72" spans="1:10" ht="22">
       <c r="A72" s="3" t="s">
         <v>12</v>
       </c>
@@ -2662,7 +2749,7 @@
       <c r="C72" s="3">
         <v>0</v>
       </c>
-      <c r="D72" s="13"/>
+      <c r="D72" s="11"/>
       <c r="E72" s="3">
         <v>0</v>
       </c>
@@ -2670,102 +2757,102 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="14"/>
-    </row>
-    <row r="73" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A73" s="62" t="s">
+      <c r="J72" s="12"/>
+    </row>
+    <row r="73" spans="1:10" ht="22">
+      <c r="A73" s="55" t="s">
         <v>21</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="46">
+      <c r="C73" s="18">
         <f>SUM(C67:C72)</f>
         <v>7.96</v>
       </c>
-      <c r="D73" s="47">
+      <c r="D73" s="19">
         <f>SUM(D67:D72)</f>
         <v>20.81</v>
       </c>
-      <c r="E73" s="48">
+      <c r="E73" s="20">
         <f>SUM(E67:E72)</f>
         <v>15.370000000000001</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="19" t="s">
+      <c r="G73" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H73" s="20"/>
-      <c r="I73" s="20"/>
-      <c r="J73" s="21"/>
-    </row>
-    <row r="74" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A74" s="63"/>
-      <c r="B74" s="23" t="s">
+      <c r="H73" s="34"/>
+      <c r="I73" s="34"/>
+      <c r="J73" s="35"/>
+    </row>
+    <row r="74" spans="1:10" ht="22">
+      <c r="A74" s="56"/>
+      <c r="B74" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C74" s="49">
+      <c r="C74" s="57">
         <f>SUM(C73:E73)</f>
         <v>44.14</v>
       </c>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="51"/>
-      <c r="G74" s="19">
+      <c r="D74" s="58"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="33">
         <f>ROUNDUP(SUM(C73:E73)/3,2)</f>
         <v>14.72</v>
       </c>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="21"/>
-    </row>
-    <row r="75" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
-      <c r="B75" s="73" t="s">
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="35"/>
+    </row>
+    <row r="75" spans="1:10" ht="22" customHeight="1">
+      <c r="A75" s="47"/>
+      <c r="B75" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C75" s="53">
+      <c r="C75" s="49">
         <f>SUM(C62+C74)</f>
         <v>85.2</v>
       </c>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="53">
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="49">
         <f>SUM(G62+G74)</f>
         <v>28.41</v>
       </c>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
-      <c r="J75" s="55"/>
-    </row>
-    <row r="76" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="56"/>
-      <c r="B76" s="74"/>
-      <c r="C76" s="57"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
-      <c r="F76" s="59"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="59"/>
-    </row>
-    <row r="77" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A77" s="11"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="44"/>
-    </row>
-    <row r="78" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H75" s="50"/>
+      <c r="I75" s="50"/>
+      <c r="J75" s="51"/>
+    </row>
+    <row r="76" spans="1:10" ht="22" customHeight="1">
+      <c r="A76" s="48"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="52"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="54"/>
+    </row>
+    <row r="77" spans="1:10" s="76" customFormat="1" ht="11">
+      <c r="A77" s="73"/>
+      <c r="B77" s="74"/>
+      <c r="C77" s="74"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="74"/>
+      <c r="H77" s="74"/>
+      <c r="I77" s="74"/>
+      <c r="J77" s="75"/>
+    </row>
+    <row r="78" spans="1:10" ht="22">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -2793,14 +2880,14 @@
       <c r="I78" s="8"/>
       <c r="J78" s="9"/>
     </row>
-    <row r="79" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="22">
       <c r="A79" s="10"/>
       <c r="B79" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="11"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
       <c r="F79" s="3" t="s">
         <v>9</v>
       </c>
@@ -2817,7 +2904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="22">
       <c r="A80" s="4"/>
       <c r="B80" s="3">
         <v>1</v>
@@ -2828,19 +2915,19 @@
       <c r="D80" s="4">
         <v>0</v>
       </c>
-      <c r="E80" s="13"/>
+      <c r="E80" s="11"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="14"/>
-    </row>
-    <row r="81" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J80" s="12"/>
+    </row>
+    <row r="81" spans="1:10" ht="22">
       <c r="A81" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B81" s="3">
         <v>2</v>
       </c>
-      <c r="C81" s="13"/>
+      <c r="C81" s="11"/>
       <c r="D81" s="4">
         <v>4.74</v>
       </c>
@@ -2855,9 +2942,9 @@
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="14"/>
-    </row>
-    <row r="82" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J81" s="12"/>
+    </row>
+    <row r="82" spans="1:10" ht="22">
       <c r="A82" s="3" t="s">
         <v>11</v>
       </c>
@@ -2867,7 +2954,7 @@
       <c r="C82" s="4">
         <v>4.74</v>
       </c>
-      <c r="D82" s="13"/>
+      <c r="D82" s="11"/>
       <c r="E82" s="4">
         <v>4.74</v>
       </c>
@@ -2879,9 +2966,9 @@
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="14"/>
-    </row>
-    <row r="83" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J82" s="12"/>
+    </row>
+    <row r="83" spans="1:10" ht="22">
       <c r="A83" s="4"/>
       <c r="B83" s="3">
         <v>4</v>
@@ -2892,19 +2979,19 @@
       <c r="D83" s="4">
         <v>2.16</v>
       </c>
-      <c r="E83" s="13"/>
-      <c r="F83" s="64">
+      <c r="E83" s="11"/>
+      <c r="F83" s="23">
         <v>413</v>
       </c>
-      <c r="G83" s="64"/>
-      <c r="J83" s="14"/>
-    </row>
-    <row r="84" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="G83" s="23"/>
+      <c r="J83" s="12"/>
+    </row>
+    <row r="84" spans="1:10" ht="22">
       <c r="A84" s="4"/>
       <c r="B84" s="3">
         <v>5</v>
       </c>
-      <c r="C84" s="13"/>
+      <c r="C84" s="11"/>
       <c r="D84" s="4">
         <v>0</v>
       </c>
@@ -2915,9 +3002,9 @@
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
-      <c r="J84" s="14"/>
-    </row>
-    <row r="85" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J84" s="12"/>
+    </row>
+    <row r="85" spans="1:10" ht="22">
       <c r="A85" s="3" t="s">
         <v>12</v>
       </c>
@@ -2927,7 +3014,7 @@
       <c r="C85" s="4">
         <v>4.53</v>
       </c>
-      <c r="D85" s="13"/>
+      <c r="D85" s="11"/>
       <c r="E85" s="4">
         <v>4.53</v>
       </c>
@@ -2939,100 +3026,100 @@
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="14"/>
-    </row>
-    <row r="86" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A86" s="67" t="s">
+      <c r="J85" s="12"/>
+    </row>
+    <row r="86" spans="1:10" ht="22">
+      <c r="A86" s="60" t="s">
         <v>23</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C86" s="16">
+      <c r="C86" s="13">
         <f>SUM(C80:C85)</f>
         <v>11.43</v>
       </c>
-      <c r="D86" s="17">
+      <c r="D86" s="14">
         <f>SUM(D80:D85)</f>
         <v>6.9</v>
       </c>
-      <c r="E86" s="18">
+      <c r="E86" s="15">
         <f>SUM(E80:E85)</f>
         <v>14.010000000000002</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G86" s="19" t="s">
+      <c r="G86" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H86" s="20"/>
-      <c r="I86" s="20"/>
-      <c r="J86" s="21"/>
-    </row>
-    <row r="87" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A87" s="68"/>
-      <c r="B87" s="23" t="s">
+      <c r="H86" s="34"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="35"/>
+    </row>
+    <row r="87" spans="1:10" ht="24">
+      <c r="A87" s="61"/>
+      <c r="B87" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C87" s="24">
+      <c r="C87" s="70">
         <f>SUM(C86:E86)</f>
         <v>32.340000000000003</v>
       </c>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="27">
+      <c r="D87" s="71"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="72"/>
+      <c r="G87" s="36">
         <f>ROUNDUP(SUM(C86:E86)/3,2)</f>
         <v>10.78</v>
       </c>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-      <c r="J87" s="29"/>
-    </row>
-    <row r="88" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="30"/>
-      <c r="B88" s="75"/>
-      <c r="C88" s="31">
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="38"/>
+    </row>
+    <row r="88" spans="1:10" ht="22" customHeight="1">
+      <c r="A88" s="39"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="64">
         <f>C87</f>
         <v>32.340000000000003</v>
       </c>
-      <c r="D88" s="32"/>
-      <c r="E88" s="32"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="34">
+      <c r="D88" s="65"/>
+      <c r="E88" s="65"/>
+      <c r="F88" s="66"/>
+      <c r="G88" s="41">
         <f>G87</f>
         <v>10.78</v>
       </c>
-      <c r="H88" s="35"/>
-      <c r="I88" s="35"/>
-      <c r="J88" s="36"/>
-    </row>
-    <row r="89" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="75"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="41"/>
-      <c r="H89" s="42"/>
-      <c r="I89" s="42"/>
-      <c r="J89" s="43"/>
-    </row>
-    <row r="90" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A90" s="11"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
-      <c r="J90" s="44"/>
-    </row>
-    <row r="91" spans="1:10" ht="22" x14ac:dyDescent="0.2">
+      <c r="H88" s="42"/>
+      <c r="I88" s="42"/>
+      <c r="J88" s="43"/>
+    </row>
+    <row r="89" spans="1:10" ht="22" customHeight="1">
+      <c r="A89" s="40"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="67"/>
+      <c r="D89" s="68"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="69"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="45"/>
+      <c r="I89" s="45"/>
+      <c r="J89" s="46"/>
+    </row>
+    <row r="90" spans="1:10" s="80" customFormat="1" ht="7">
+      <c r="A90" s="77"/>
+      <c r="B90" s="78"/>
+      <c r="C90" s="78"/>
+      <c r="D90" s="78"/>
+      <c r="E90" s="78"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="78"/>
+      <c r="H90" s="78"/>
+      <c r="I90" s="78"/>
+      <c r="J90" s="79"/>
+    </row>
+    <row r="91" spans="1:10" ht="22">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
@@ -3060,14 +3147,14 @@
       <c r="I91" s="8"/>
       <c r="J91" s="9"/>
     </row>
-    <row r="92" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A92" s="45"/>
+    <row r="92" spans="1:10" ht="22">
+      <c r="A92" s="17"/>
       <c r="B92" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
       <c r="F92" s="3" t="s">
         <v>9</v>
       </c>
@@ -3080,11 +3167,11 @@
       <c r="I92" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J92" s="60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J92" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="22">
       <c r="A93" s="4"/>
       <c r="B93" s="3">
         <v>1</v>
@@ -3095,7 +3182,7 @@
       <c r="D93" s="3">
         <v>4.74</v>
       </c>
-      <c r="E93" s="13"/>
+      <c r="E93" s="11"/>
       <c r="F93" s="4">
         <v>731</v>
       </c>
@@ -3104,16 +3191,16 @@
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
-      <c r="J93" s="14"/>
-    </row>
-    <row r="94" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J93" s="12"/>
+    </row>
+    <row r="94" spans="1:10" ht="22">
       <c r="A94" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B94" s="3">
         <v>2</v>
       </c>
-      <c r="C94" s="13"/>
+      <c r="C94" s="11"/>
       <c r="D94" s="3">
         <v>0</v>
       </c>
@@ -3122,9 +3209,9 @@
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
-      <c r="J94" s="14"/>
-    </row>
-    <row r="95" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J94" s="12"/>
+    </row>
+    <row r="95" spans="1:10" ht="22">
       <c r="A95" s="3" t="s">
         <v>11</v>
       </c>
@@ -3134,7 +3221,7 @@
       <c r="C95" s="3">
         <v>4.53</v>
       </c>
-      <c r="D95" s="13"/>
+      <c r="D95" s="11"/>
       <c r="E95" s="3">
         <v>4.53</v>
       </c>
@@ -3146,9 +3233,9 @@
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
-      <c r="J95" s="14"/>
-    </row>
-    <row r="96" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J95" s="12"/>
+    </row>
+    <row r="96" spans="1:10" ht="22">
       <c r="A96" s="4"/>
       <c r="B96" s="3">
         <v>4</v>
@@ -3159,19 +3246,19 @@
       <c r="D96" s="3">
         <v>0</v>
       </c>
-      <c r="E96" s="13"/>
+      <c r="E96" s="11"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
-      <c r="J96" s="14"/>
-    </row>
-    <row r="97" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J96" s="12"/>
+    </row>
+    <row r="97" spans="1:10" ht="22">
       <c r="A97" s="4"/>
       <c r="B97" s="3">
         <v>5</v>
       </c>
-      <c r="C97" s="13"/>
+      <c r="C97" s="11"/>
       <c r="D97" s="3">
         <v>0</v>
       </c>
@@ -3182,9 +3269,9 @@
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
-      <c r="J97" s="14"/>
-    </row>
-    <row r="98" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="J97" s="12"/>
+    </row>
+    <row r="98" spans="1:10" ht="22">
       <c r="A98" s="3" t="s">
         <v>12</v>
       </c>
@@ -3194,7 +3281,7 @@
       <c r="C98" s="3">
         <v>4.74</v>
       </c>
-      <c r="D98" s="13"/>
+      <c r="D98" s="11"/>
       <c r="E98" s="3">
         <v>4.74</v>
       </c>
@@ -3206,133 +3293,140 @@
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
-      <c r="J98" s="14"/>
-    </row>
-    <row r="99" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A99" s="67" t="s">
+      <c r="J98" s="12"/>
+    </row>
+    <row r="99" spans="1:10" ht="22">
+      <c r="A99" s="60" t="s">
         <v>24</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C99" s="46">
+      <c r="C99" s="18">
         <f>SUM(C93:C98)</f>
         <v>14.01</v>
       </c>
-      <c r="D99" s="47">
+      <c r="D99" s="19">
         <f>SUM(D93:D98)</f>
         <v>4.74</v>
       </c>
-      <c r="E99" s="48">
+      <c r="E99" s="20">
         <f>SUM(E93:E98)</f>
         <v>9.27</v>
       </c>
       <c r="F99" s="3"/>
-      <c r="G99" s="19" t="s">
+      <c r="G99" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H99" s="20"/>
-      <c r="I99" s="20"/>
-      <c r="J99" s="21"/>
-    </row>
-    <row r="100" spans="1:10" ht="22" x14ac:dyDescent="0.2">
-      <c r="A100" s="68"/>
-      <c r="B100" s="23" t="s">
+      <c r="H99" s="34"/>
+      <c r="I99" s="34"/>
+      <c r="J99" s="35"/>
+    </row>
+    <row r="100" spans="1:10" ht="22">
+      <c r="A100" s="61"/>
+      <c r="B100" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C100" s="49">
+      <c r="C100" s="57">
         <f>SUM(C99:E99)</f>
         <v>28.02</v>
       </c>
-      <c r="D100" s="50"/>
-      <c r="E100" s="50"/>
-      <c r="F100" s="51"/>
-      <c r="G100" s="19">
+      <c r="D100" s="58"/>
+      <c r="E100" s="58"/>
+      <c r="F100" s="59"/>
+      <c r="G100" s="33">
         <f>ROUNDUP(SUM(C99:E99)/3,2)</f>
         <v>9.34</v>
       </c>
-      <c r="H100" s="20"/>
-      <c r="I100" s="20"/>
-      <c r="J100" s="21"/>
-    </row>
-    <row r="101" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="52"/>
-      <c r="B101" s="73" t="s">
+      <c r="H100" s="34"/>
+      <c r="I100" s="34"/>
+      <c r="J100" s="35"/>
+    </row>
+    <row r="101" spans="1:10" ht="22" customHeight="1">
+      <c r="A101" s="47"/>
+      <c r="B101" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C101" s="53">
+      <c r="C101" s="49">
         <f>SUM(C88+C100)</f>
         <v>60.36</v>
       </c>
-      <c r="D101" s="54"/>
-      <c r="E101" s="54"/>
-      <c r="F101" s="55"/>
-      <c r="G101" s="53">
+      <c r="D101" s="50"/>
+      <c r="E101" s="50"/>
+      <c r="F101" s="51"/>
+      <c r="G101" s="49">
         <f>SUM(G88+G100)</f>
         <v>20.119999999999997</v>
       </c>
-      <c r="H101" s="54"/>
-      <c r="I101" s="54"/>
-      <c r="J101" s="55"/>
-    </row>
-    <row r="102" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="56"/>
-      <c r="B102" s="74"/>
-      <c r="C102" s="57"/>
-      <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="59"/>
-      <c r="G102" s="57"/>
-      <c r="H102" s="58"/>
-      <c r="I102" s="58"/>
-      <c r="J102" s="59"/>
-    </row>
-    <row r="103" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A103" s="69" t="s">
+      <c r="H101" s="50"/>
+      <c r="I101" s="50"/>
+      <c r="J101" s="51"/>
+    </row>
+    <row r="102" spans="1:10" ht="22" customHeight="1">
+      <c r="A102" s="48"/>
+      <c r="B102" s="63"/>
+      <c r="C102" s="52"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="54"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="53"/>
+      <c r="I102" s="53"/>
+      <c r="J102" s="54"/>
+    </row>
+    <row r="103" spans="1:10" ht="22" customHeight="1">
+      <c r="A103" s="81"/>
+      <c r="B103" s="82"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="83"/>
+      <c r="G103" s="83"/>
+      <c r="H103" s="83"/>
+      <c r="I103" s="83"/>
+      <c r="J103" s="83"/>
+    </row>
+    <row r="104" spans="1:10" s="91" customFormat="1" ht="32">
+      <c r="A104" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B103" s="70"/>
-      <c r="C103" s="46">
+      <c r="B104" s="85"/>
+      <c r="C104" s="86">
         <f>SUM(C9+C22+C34+C47+C60+C73+C86+C99)</f>
         <v>110.46</v>
       </c>
-      <c r="D103" s="47">
+      <c r="D104" s="87">
         <f>SUM(D9+D22+D34+D47+D60+D73+D86+D99)</f>
         <v>113.32000000000001</v>
       </c>
-      <c r="E103" s="48">
+      <c r="E104" s="88">
         <f>SUM(E9+E22+E34+E47+E60+E73+E86+E99)</f>
         <v>107.98000000000002</v>
       </c>
-      <c r="F103" s="71" t="s">
+      <c r="F104" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="G103" s="72"/>
-      <c r="H103" s="72"/>
-      <c r="I103" s="72"/>
-      <c r="J103" s="72"/>
+      <c r="G104" s="90"/>
+      <c r="H104" s="90"/>
+      <c r="I104" s="90"/>
+      <c r="J104" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C61:F61"/>
-    <mergeCell ref="C62:F63"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C88:F89"/>
-    <mergeCell ref="C87:F87"/>
-    <mergeCell ref="C75:F76"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F12"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="C24:F25"/>
     <mergeCell ref="C35:F35"/>
     <mergeCell ref="C36:F37"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="A101:A102"/>
     <mergeCell ref="G101:J102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="F103:J103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="F104:J104"/>
     <mergeCell ref="C101:F102"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="A88:A89"/>
@@ -3343,6 +3437,7 @@
     <mergeCell ref="G99:J99"/>
     <mergeCell ref="G100:J100"/>
     <mergeCell ref="C100:F100"/>
+    <mergeCell ref="C88:F89"/>
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="G75:J76"/>
     <mergeCell ref="A77:J77"/>
@@ -3350,6 +3445,9 @@
     <mergeCell ref="A86:A87"/>
     <mergeCell ref="G86:J86"/>
     <mergeCell ref="G87:J87"/>
+    <mergeCell ref="C87:F87"/>
+    <mergeCell ref="C75:F76"/>
+    <mergeCell ref="B75:B76"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="G62:J63"/>
     <mergeCell ref="A64:J64"/>
@@ -3357,6 +3455,8 @@
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="G73:J73"/>
     <mergeCell ref="G74:J74"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C62:F63"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="G49:J50"/>
     <mergeCell ref="A51:J51"/>
@@ -3365,6 +3465,8 @@
     <mergeCell ref="G60:J60"/>
     <mergeCell ref="G61:J61"/>
     <mergeCell ref="C49:F50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C61:F61"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="G36:J37"/>
     <mergeCell ref="A38:J38"/>
@@ -3379,34 +3481,32 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="G35:J35"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="G11:J12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5F4B6F-0E31-7948-9A9F-67C9D04FB46F}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3416,8 +3516,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <f>INT(0)</f>
         <v>0</v>
@@ -3429,8 +3532,12 @@
       <c r="C2">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="25">
+        <f>Racks!H1</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>100</v>
       </c>
@@ -3440,8 +3547,12 @@
       <c r="C3" s="2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="25">
+        <f>Racks!H14</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>200</v>
       </c>
@@ -3451,8 +3562,12 @@
       <c r="C4">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="25">
+        <f>Racks!H26</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>300</v>
       </c>
@@ -3462,8 +3577,12 @@
       <c r="C5">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="25">
+        <f>Racks!H39</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>400</v>
       </c>
@@ -3473,8 +3592,12 @@
       <c r="C6">
         <v>820</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="25">
+        <f>Racks!H52</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>500</v>
       </c>
@@ -3484,8 +3607,12 @@
       <c r="C7">
         <v>582</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="25">
+        <f>Racks!H65</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>600</v>
       </c>
@@ -3495,8 +3622,12 @@
       <c r="C8">
         <v>350</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="25">
+        <f>Racks!H78</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>700</v>
       </c>
@@ -3506,8 +3637,12 @@
       <c r="C9">
         <v>900</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="25">
+        <f>Racks!H91</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>800</v>
       </c>
@@ -3518,7 +3653,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>900</v>
       </c>
@@ -3529,7 +3664,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1000</v>
       </c>
@@ -3540,7 +3675,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1100</v>
       </c>
@@ -3563,7 +3698,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>